<commit_message>
Policy Creation script completed
</commit_message>
<xml_diff>
--- a/Data/ConfigData/PolicyConfig.xlsx
+++ b/Data/ConfigData/PolicyConfig.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4347C0A-592F-49FF-8939-F74148A2D731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F3172-AB30-4BA0-B901-EFF7012DD1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewPolicy" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>FarmerRegData</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>ResNewPolicy</t>
+  </si>
+  <si>
+    <t>newpol_002</t>
   </si>
 </sst>
 </file>
@@ -506,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,9 +643,59 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+      <c r="U3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DN & OR is implemented
</commit_message>
<xml_diff>
--- a/Data/ConfigData/PolicyConfig.xlsx
+++ b/Data/ConfigData/PolicyConfig.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F3172-AB30-4BA0-B901-EFF7012DD1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBF00C8-B898-4B2B-90DA-3FF756789C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewPolicy" sheetId="1" r:id="rId1"/>
-    <sheet name="EditPolicy" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
-  <si>
-    <t>FarmerRegData</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TestDataFile</t>
   </si>
@@ -42,9 +38,6 @@
     <t>ResSheet</t>
   </si>
   <si>
-    <t>ResFarmerReg</t>
-  </si>
-  <si>
     <t>DepChkFile</t>
   </si>
   <si>
@@ -85,24 +78,6 @@
   </si>
   <si>
     <t>DepChkDepValCol</t>
-  </si>
-  <si>
-    <t>DepFarmerReg</t>
-  </si>
-  <si>
-    <t>fmodreg_001</t>
-  </si>
-  <si>
-    <t>Modify farmer name</t>
-  </si>
-  <si>
-    <t>ModReg</t>
-  </si>
-  <si>
-    <t>To check for basic modification end date</t>
-  </si>
-  <si>
-    <t>fmodreg_018</t>
   </si>
   <si>
     <t>newpol_001</t>
@@ -536,87 +511,87 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -628,10 +603,10 @@
         <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="Q2">
         <v>4</v>
@@ -651,22 +626,22 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L3">
         <v>4</v>
@@ -678,10 +653,10 @@
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="Q3">
         <v>4</v>
@@ -730,205 +705,6 @@
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
-    <col min="16" max="19" width="8.88671875" customWidth="1"/>
-    <col min="20" max="20" width="13" customWidth="1"/>
-    <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2">
-        <v>4</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="O3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>8</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>